<commit_message>
Standardizing format for testing
</commit_message>
<xml_diff>
--- a/tests/files/example_xlsx.xlsx
+++ b/tests/files/example_xlsx.xlsx
@@ -12,23 +12,23 @@
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
-    <sheet name="current" sheetId="33" r:id="rId1"/>
+    <sheet name="Current Schedule" sheetId="33" r:id="rId1"/>
     <sheet name="Starting January 1, 2001" sheetId="45" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">current!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Current Schedule'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Starting January 1, 2001'!$A$460:$G$592</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">current!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Current Schedule'!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Starting January 1, 2001'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
+    <customWorkbookView name="ds - Personal View" guid="{36D7B830-3C20-4BDC-A569-E6D13D954A90}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1148" windowHeight="643" activeSheetId="3"/>
+    <customWorkbookView name="sh - Personal View" guid="{8361DC2F-A38F-46D3-91A4-E5FE7A212FA0}" mergeInterval="0" personalView="1" maximized="1" windowWidth="794" windowHeight="433" activeSheetId="3" showComments="commIndAndComment"/>
+    <customWorkbookView name="Administrator - Personal View" guid="{F3202F01-C0D3-43F7-BE44-8DBEA389C46F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="767" windowHeight="467" activeSheetId="3" showComments="commNone"/>
+    <customWorkbookView name="RMC - Personal View" guid="{943740EF-F889-4052-9641-C36AEC0D3C9F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="987" windowHeight="606" activeSheetId="3"/>
+    <customWorkbookView name="Ian Creurer - Personal View" guid="{0E505AFB-BF15-4A62-9FB0-B8CE9D65EE8D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="987" windowHeight="606" activeSheetId="3"/>
     <customWorkbookView name="DTHR - Personal View" guid="{3345313B-C5E2-4C0C-BD52-39D40835B2D0}" mergeInterval="0" personalView="1" maximized="1" windowWidth="794" windowHeight="433" activeSheetId="3"/>
-    <customWorkbookView name="Ian Creurer - Personal View" guid="{0E505AFB-BF15-4A62-9FB0-B8CE9D65EE8D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="987" windowHeight="606" activeSheetId="3"/>
-    <customWorkbookView name="RMC - Personal View" guid="{943740EF-F889-4052-9641-C36AEC0D3C9F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="987" windowHeight="606" activeSheetId="3"/>
-    <customWorkbookView name="Administrator - Personal View" guid="{F3202F01-C0D3-43F7-BE44-8DBEA389C46F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="767" windowHeight="467" activeSheetId="3" showComments="commNone"/>
-    <customWorkbookView name="sh - Personal View" guid="{8361DC2F-A38F-46D3-91A4-E5FE7A212FA0}" mergeInterval="0" personalView="1" maximized="1" windowWidth="794" windowHeight="433" activeSheetId="3" showComments="commIndAndComment"/>
-    <customWorkbookView name="ds - Personal View" guid="{36D7B830-3C20-4BDC-A569-E6D13D954A90}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1148" windowHeight="643" activeSheetId="3"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -7164,7 +7164,7 @@
     <outlinePr showOutlineSymbols="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD368"/>
+  <dimension ref="A1:G368"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="20" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D356" activePane="bottomRight" state="frozen"/>
@@ -13691,7 +13691,7 @@
     <outlinePr showOutlineSymbols="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BM635"/>
+  <dimension ref="A1:G635"/>
   <sheetViews>
     <sheetView showOutlineSymbols="0" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="20" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D363" activePane="bottomRight" state="frozen"/>
@@ -13700,7 +13700,7 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5:B375"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.450000000000003" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.450000000000003" customHeight="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -20589,29 +20589,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <Area_x0020_of_x0020_Operations xmlns="37637be6-5d3e-457d-a64b-37b5e88ebe78">Central Zone - Red Deer</Area_x0020_of_x0020_Operations>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="be7adf94-23b5-4e04-9f58-6bdd5e5a7df3" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F050D63782F87D4CA7C5F6012DEA5F01" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="42091815ee4495d25e0cb9d6d7529466">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns3="37637be6-5d3e-457d-a64b-37b5e88ebe78" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f21679de478cb3e0b666abb9acaccf7" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -20755,6 +20732,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="be7adf94-23b5-4e04-9f58-6bdd5e5a7df3" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <Area_x0020_of_x0020_Operations xmlns="37637be6-5d3e-457d-a64b-37b5e88ebe78">Central Zone - Red Deer</Area_x0020_of_x0020_Operations>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D666DB61-1780-444E-A832-F56B634C65A2}">
   <ds:schemaRefs>
@@ -20764,39 +20764,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C97C5340-9F2C-412E-9F78-96206CE52560}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="37637be6-5d3e-457d-a64b-37b5e88ebe78"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC1A97E-FB5C-45B1-8B61-C46413129570}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4F8251C-14AE-4D2C-9E03-8073CD84BBE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1860063-7891-477D-B892-D36A0028708B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20813,4 +20780,37 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4F8251C-14AE-4D2C-9E03-8073CD84BBE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC1A97E-FB5C-45B1-8B61-C46413129570}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C97C5340-9F2C-412E-9F78-96206CE52560}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="37637be6-5d3e-457d-a64b-37b5e88ebe78"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>